<commit_message>
register student excel file is done
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,132 +458,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>92310133004</t>
+          <t>92200133003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bhargav_1</t>
+          <t>Prashant_1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>06:09:07</t>
+          <t>18:27:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>922001330003</t>
+          <t>92200133031</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Prashnat_1</t>
+          <t>Kirtan_1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>05:10:10</t>
+          <t>18:26:43</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>92200133022</t>
+          <t>92310133004</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Krish_1</t>
+          <t>Bhargav_1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-04</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05:10:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>92200133030</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Aryan_Langhanoja_1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>05:10:55</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>92200133031</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Kritan_1</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>05:11:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>922310133004</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Bhargav_1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-08-28</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>05:11:32</t>
+          <t>18:26:14</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Student Excel Sheet
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -7,7 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="All Students" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="1234-1234" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2025-2026" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2025-2027" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +20,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +45,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,90 +425,249 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Batch Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>ER Number</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Student Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Upload Date</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Upload Time</t>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Upload Date &amp; Time</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>92200133003</t>
+          <t>1234-1234</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Prashant_1</t>
+          <t>92310133004</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>Bhargav_1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>18:27:00</t>
+          <t>2025-09-07 12:17:35</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>92200133031</t>
+          <t>2025-2026</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kirtan_1</t>
+          <t>92310133004</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-09-04</t>
+          <t>Bhargav_1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18:26:43</t>
+          <t>2025-09-07 12:17:42</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>2025-2027</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>92310133004</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Bhargav_1</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-09-04</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18:26:14</t>
+          <t>2025-09-07 12:19:09</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ER Number</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Student Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Upload Date &amp; Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>92310133004</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bhargav_1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-09-07 12:17:35</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ER Number</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Student Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Upload Date &amp; Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>92310133004</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bhargav_1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-09-07 12:17:42</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ER Number</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Student Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Upload Date &amp; Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>92310133004</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bhargav_1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-09-07 12:19:09</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add rekognition function with update
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="All Students" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="1234-1234" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2025-2026" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="2025-2027" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2022-2026" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,61 +453,105 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>92310133004</t>
+          <t>1233123</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bhargav_1</t>
+          <t>qwe_1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-09-07 12:17:35</t>
+          <t>2025-09-18 04:59:49</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-2026</t>
+          <t>1234-1234</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>92310133004</t>
+          <t>92200133031</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bhargav_1</t>
+          <t>Kirtan_1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-09-07 12:17:42</t>
+          <t>2025-09-18 05:14:31</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-2027</t>
+          <t>2022-2026</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>92200133003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Prashant_1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:52:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2022-2026</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>92310133004</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Bhargav_1</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-09-07 12:19:09</t>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:51:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2022-2026</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>92310133019</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Neel_1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:52:16</t>
         </is>
       </c>
     </row>
@@ -523,7 +566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,17 +594,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>92310133004</t>
+          <t>1233123</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bhargav_1</t>
+          <t>qwe_1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-09-07 12:17:35</t>
+          <t>2025-09-18 04:59:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>92200133031</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Kirtan_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-09-18 05:14:31</t>
         </is>
       </c>
     </row>
@@ -576,7 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,70 +664,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>92200133003</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Prashant_1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:52:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>92310133004</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Bhargav_1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-09-07 12:17:42</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ER Number</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Student Name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Upload Date &amp; Time</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>92310133004</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Bhargav_1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-09-07 12:19:09</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:51:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>92310133019</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Neel_1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-09-18 04:52:16</t>
         </is>
       </c>
     </row>

</xml_diff>